<commit_message>
Update project qustions code
</commit_message>
<xml_diff>
--- a/Corelation.xlsx
+++ b/Corelation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koutn\sql-repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565CBA8F-72DA-4246-B159-3C8590D70B11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D1AADA-5A5E-43E5-B03C-EC67156DD3BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>Year</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Souvislost mezi růstem mezd v následujícím roce a HDP ve předchozím roce</t>
+  </si>
+  <si>
+    <t>Korelačni koeficient mezi růstem mezd a HDP pouze pro HDP &gt; 5%</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -993,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M1"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1014,24 +1017,32 @@
     <col min="18" max="18" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="H1" s="6" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="P1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1074,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2001</v>
       </c>
@@ -1109,7 +1120,7 @@
         <v>6.6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2002</v>
       </c>
@@ -1144,7 +1155,7 @@
         <v>6.77</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2003</v>
       </c>
@@ -1180,7 +1191,7 @@
         <v>5.57</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>2004</v>
       </c>
@@ -1215,7 +1226,7 @@
         <v>5.39</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2005</v>
       </c>
@@ -1250,7 +1261,7 @@
         <v>5.17</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2006</v>
       </c>
@@ -1276,7 +1287,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>2007</v>
       </c>
@@ -1309,7 +1320,7 @@
         <v>0.3121413720039109</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>2008</v>
       </c>
@@ -1336,7 +1347,7 @@
       </c>
       <c r="R10" s="5"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>2009</v>
       </c>
@@ -1363,7 +1374,7 @@
       </c>
       <c r="R11" s="5"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>2010</v>
       </c>
@@ -1388,8 +1399,16 @@
         <f t="shared" si="1"/>
         <v>2009</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="P12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>2011</v>
       </c>
@@ -1427,7 +1446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>2012</v>
       </c>
@@ -1466,7 +1485,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>2013</v>
       </c>
@@ -1505,7 +1524,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>2014</v>
       </c>
@@ -1743,9 +1762,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="H1:M1"/>
+    <mergeCell ref="P1:U1"/>
+    <mergeCell ref="P12:U12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>